<commit_message>
update report cell style
</commit_message>
<xml_diff>
--- a/School.Financial/ReportSrc/chequereport.xlsx
+++ b/School.Financial/ReportSrc/chequereport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="83">
   <si>
     <r>
       <t xml:space="preserve">ฉบับที่ 1 </t>
@@ -411,9 +411,6 @@
   </si>
   <si>
     <t>{amountbefore}</t>
-  </si>
-  <si>
-    <t>{vat}</t>
   </si>
   <si>
     <t>(เช่น รางวัล ส่วนลดหรือประโยชน์ใดๆ เนื่องจากการส่งเสริมการขาย รางวัลในการประกวด การแข่งขัน การชิงโชค ค่าแสดงของนักแสดงสาธารณะ ค่าจ้างทำของ ค่าโฆษณา ค่าเช่า ค่าขนส่ง ค่าบริการ ค่าเบี้ยประกันวินาศภัย ฯลฯ)</t>
@@ -1329,6 +1326,158 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="167" fontId="22" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1368,9 +1517,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1416,155 +1562,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1603,7 +1600,7 @@
         <xdr:cNvPr id="3" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1300-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1659,7 +1656,7 @@
         <xdr:cNvPr id="2" name="Rectangle 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1300-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2023,7 +2020,7 @@
   <dimension ref="A1:S68"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U49" sqref="U49"/>
+      <selection activeCell="V46" sqref="V46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,23 +2079,23 @@
     </row>
     <row r="3" spans="1:19" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="162" t="s">
+      <c r="B3" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="162"/>
-      <c r="M3" s="162"/>
-      <c r="N3" s="162"/>
-      <c r="O3" s="162"/>
-      <c r="P3" s="162"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
+      <c r="K3" s="128"/>
+      <c r="L3" s="128"/>
+      <c r="M3" s="128"/>
+      <c r="N3" s="128"/>
+      <c r="O3" s="128"/>
+      <c r="P3" s="128"/>
       <c r="Q3" s="5" t="s">
         <v>3</v>
       </c>
@@ -2106,28 +2103,28 @@
         <v>4</v>
       </c>
       <c r="S3" s="104" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="163"/>
-      <c r="J4" s="163"/>
-      <c r="K4" s="163"/>
-      <c r="L4" s="163"/>
-      <c r="M4" s="163"/>
-      <c r="N4" s="163"/>
-      <c r="O4" s="163"/>
-      <c r="P4" s="163"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="129"/>
+      <c r="N4" s="129"/>
+      <c r="O4" s="129"/>
+      <c r="P4" s="129"/>
       <c r="Q4" s="8" t="s">
         <v>6</v>
       </c>
@@ -2167,17 +2164,17 @@
         <v>10</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="164" t="s">
+      <c r="D6" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="164"/>
-      <c r="F6" s="164"/>
-      <c r="G6" s="164"/>
-      <c r="H6" s="164"/>
-      <c r="I6" s="164"/>
-      <c r="J6" s="164"/>
-      <c r="K6" s="164"/>
-      <c r="L6" s="164"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="130"/>
       <c r="M6" s="17" t="s">
         <v>12</v>
       </c>
@@ -2185,10 +2182,10 @@
       <c r="O6" s="18"/>
       <c r="P6" s="18"/>
       <c r="Q6" s="18"/>
-      <c r="R6" s="182" t="s">
+      <c r="R6" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="S6" s="185"/>
+      <c r="S6" s="111"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
@@ -2213,7 +2210,7 @@
       <c r="R7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="S7" s="186"/>
+      <c r="S7" s="112"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -2221,23 +2218,23 @@
         <v>16</v>
       </c>
       <c r="C8" s="16"/>
-      <c r="D8" s="164" t="s">
+      <c r="D8" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="164"/>
-      <c r="H8" s="164"/>
-      <c r="I8" s="164"/>
-      <c r="J8" s="164"/>
-      <c r="K8" s="164"/>
-      <c r="L8" s="164"/>
-      <c r="M8" s="164"/>
-      <c r="N8" s="164"/>
-      <c r="O8" s="164"/>
-      <c r="P8" s="164"/>
-      <c r="Q8" s="164"/>
-      <c r="R8" s="165"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="130"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="130"/>
+      <c r="N8" s="130"/>
+      <c r="O8" s="130"/>
+      <c r="P8" s="130"/>
+      <c r="Q8" s="130"/>
+      <c r="R8" s="131"/>
       <c r="S8" s="105"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2306,10 +2303,10 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
-      <c r="R11" s="183" t="s">
+      <c r="R11" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="S11" s="187"/>
+      <c r="S11" s="113"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
@@ -2335,10 +2332,10 @@
       <c r="O12" s="18"/>
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
-      <c r="R12" s="184" t="s">
+      <c r="R12" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="S12" s="187"/>
+      <c r="S12" s="113"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
@@ -2363,7 +2360,7 @@
       <c r="R13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="S13" s="186"/>
+      <c r="S13" s="112"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
@@ -2441,10 +2438,10 @@
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="166">
+      <c r="E17" s="132">
         <v>1</v>
       </c>
-      <c r="F17" s="167"/>
+      <c r="F17" s="133"/>
       <c r="G17" s="39"/>
       <c r="H17" s="2"/>
       <c r="I17" s="17" t="s">
@@ -2530,56 +2527,56 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="168" t="s">
+      <c r="B21" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="169"/>
-      <c r="D21" s="169"/>
-      <c r="E21" s="169"/>
-      <c r="F21" s="169"/>
-      <c r="G21" s="169"/>
-      <c r="H21" s="169"/>
-      <c r="I21" s="169"/>
-      <c r="J21" s="169"/>
-      <c r="K21" s="169"/>
-      <c r="L21" s="170"/>
-      <c r="M21" s="174" t="s">
+      <c r="C21" s="115"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="115"/>
+      <c r="G21" s="115"/>
+      <c r="H21" s="115"/>
+      <c r="I21" s="115"/>
+      <c r="J21" s="115"/>
+      <c r="K21" s="115"/>
+      <c r="L21" s="116"/>
+      <c r="M21" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="N21" s="175"/>
-      <c r="O21" s="176" t="s">
+      <c r="N21" s="121"/>
+      <c r="O21" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="177"/>
-      <c r="Q21" s="174" t="s">
+      <c r="P21" s="123"/>
+      <c r="Q21" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="R21" s="175"/>
+      <c r="R21" s="121"/>
       <c r="S21" s="105"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="171"/>
-      <c r="C22" s="172"/>
-      <c r="D22" s="172"/>
-      <c r="E22" s="172"/>
-      <c r="F22" s="172"/>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172"/>
-      <c r="J22" s="172"/>
-      <c r="K22" s="172"/>
-      <c r="L22" s="173"/>
-      <c r="M22" s="180" t="s">
+      <c r="B22" s="117"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="118"/>
+      <c r="L22" s="119"/>
+      <c r="M22" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="N22" s="181"/>
-      <c r="O22" s="178"/>
-      <c r="P22" s="179"/>
-      <c r="Q22" s="180" t="s">
+      <c r="N22" s="127"/>
+      <c r="O22" s="124"/>
+      <c r="P22" s="125"/>
+      <c r="Q22" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="R22" s="181"/>
+      <c r="R22" s="127"/>
       <c r="S22" s="105"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -2599,14 +2596,14 @@
       <c r="J23" s="22"/>
       <c r="K23" s="22"/>
       <c r="L23" s="48"/>
-      <c r="M23" s="158"/>
-      <c r="N23" s="159"/>
-      <c r="O23" s="160"/>
-      <c r="P23" s="161"/>
-      <c r="Q23" s="150">
+      <c r="M23" s="134"/>
+      <c r="N23" s="135"/>
+      <c r="O23" s="136"/>
+      <c r="P23" s="137"/>
+      <c r="Q23" s="138">
         <v>0</v>
       </c>
-      <c r="R23" s="151"/>
+      <c r="R23" s="139"/>
       <c r="S23" s="106"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -2626,14 +2623,14 @@
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
       <c r="L24" s="48"/>
-      <c r="M24" s="156"/>
-      <c r="N24" s="157"/>
-      <c r="O24" s="150"/>
-      <c r="P24" s="151"/>
-      <c r="Q24" s="150">
+      <c r="M24" s="140"/>
+      <c r="N24" s="141"/>
+      <c r="O24" s="138"/>
+      <c r="P24" s="139"/>
+      <c r="Q24" s="138">
         <v>0</v>
       </c>
-      <c r="R24" s="151"/>
+      <c r="R24" s="139"/>
       <c r="S24" s="106"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -2653,14 +2650,14 @@
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
       <c r="L25" s="48"/>
-      <c r="M25" s="156"/>
-      <c r="N25" s="157"/>
-      <c r="O25" s="150"/>
-      <c r="P25" s="151"/>
-      <c r="Q25" s="150">
+      <c r="M25" s="140"/>
+      <c r="N25" s="141"/>
+      <c r="O25" s="138"/>
+      <c r="P25" s="139"/>
+      <c r="Q25" s="138">
         <v>0</v>
       </c>
-      <c r="R25" s="151"/>
+      <c r="R25" s="139"/>
       <c r="S25" s="106"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -2680,14 +2677,14 @@
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
       <c r="L26" s="48"/>
-      <c r="M26" s="156"/>
-      <c r="N26" s="157"/>
-      <c r="O26" s="150"/>
-      <c r="P26" s="151"/>
-      <c r="Q26" s="150">
+      <c r="M26" s="140"/>
+      <c r="N26" s="141"/>
+      <c r="O26" s="138"/>
+      <c r="P26" s="139"/>
+      <c r="Q26" s="138">
         <v>0</v>
       </c>
-      <c r="R26" s="151"/>
+      <c r="R26" s="139"/>
       <c r="S26" s="106"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -2705,14 +2702,14 @@
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
       <c r="L27" s="48"/>
-      <c r="M27" s="152"/>
-      <c r="N27" s="153"/>
-      <c r="O27" s="154"/>
-      <c r="P27" s="155"/>
-      <c r="Q27" s="150">
+      <c r="M27" s="142"/>
+      <c r="N27" s="143"/>
+      <c r="O27" s="144"/>
+      <c r="P27" s="145"/>
+      <c r="Q27" s="138">
         <v>0</v>
       </c>
-      <c r="R27" s="151"/>
+      <c r="R27" s="139"/>
       <c r="S27" s="106"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2732,14 +2729,14 @@
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
       <c r="L28" s="48"/>
-      <c r="M28" s="142"/>
-      <c r="N28" s="143"/>
-      <c r="O28" s="144"/>
-      <c r="P28" s="145"/>
-      <c r="Q28" s="150">
+      <c r="M28" s="146"/>
+      <c r="N28" s="147"/>
+      <c r="O28" s="148"/>
+      <c r="P28" s="149"/>
+      <c r="Q28" s="138">
         <v>0</v>
       </c>
-      <c r="R28" s="151"/>
+      <c r="R28" s="139"/>
       <c r="S28" s="106"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -2757,14 +2754,14 @@
       <c r="J29" s="54"/>
       <c r="K29" s="54"/>
       <c r="L29" s="52"/>
-      <c r="M29" s="142"/>
-      <c r="N29" s="143"/>
-      <c r="O29" s="144"/>
-      <c r="P29" s="145"/>
-      <c r="Q29" s="150">
+      <c r="M29" s="146"/>
+      <c r="N29" s="147"/>
+      <c r="O29" s="148"/>
+      <c r="P29" s="149"/>
+      <c r="Q29" s="138">
         <v>0</v>
       </c>
-      <c r="R29" s="151"/>
+      <c r="R29" s="139"/>
       <c r="S29" s="106"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -2782,14 +2779,14 @@
       <c r="J30" s="48"/>
       <c r="K30" s="48"/>
       <c r="L30" s="52"/>
-      <c r="M30" s="146"/>
-      <c r="N30" s="147"/>
-      <c r="O30" s="148"/>
-      <c r="P30" s="149"/>
-      <c r="Q30" s="150">
+      <c r="M30" s="150"/>
+      <c r="N30" s="151"/>
+      <c r="O30" s="152"/>
+      <c r="P30" s="153"/>
+      <c r="Q30" s="138">
         <v>0</v>
       </c>
-      <c r="R30" s="151"/>
+      <c r="R30" s="139"/>
       <c r="S30" s="106"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -2807,14 +2804,14 @@
       <c r="J31" s="48"/>
       <c r="K31" s="48"/>
       <c r="L31" s="52"/>
-      <c r="M31" s="156"/>
-      <c r="N31" s="157"/>
-      <c r="O31" s="150"/>
-      <c r="P31" s="151"/>
-      <c r="Q31" s="150">
+      <c r="M31" s="140"/>
+      <c r="N31" s="141"/>
+      <c r="O31" s="138"/>
+      <c r="P31" s="139"/>
+      <c r="Q31" s="138">
         <v>0</v>
       </c>
-      <c r="R31" s="151"/>
+      <c r="R31" s="139"/>
       <c r="S31" s="106"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -2832,14 +2829,14 @@
       <c r="J32" s="48"/>
       <c r="K32" s="48"/>
       <c r="L32" s="52"/>
-      <c r="M32" s="156"/>
-      <c r="N32" s="157"/>
-      <c r="O32" s="150"/>
-      <c r="P32" s="151"/>
-      <c r="Q32" s="150">
+      <c r="M32" s="140"/>
+      <c r="N32" s="141"/>
+      <c r="O32" s="138"/>
+      <c r="P32" s="139"/>
+      <c r="Q32" s="138">
         <v>0</v>
       </c>
-      <c r="R32" s="151"/>
+      <c r="R32" s="139"/>
       <c r="S32" s="106"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -2861,14 +2858,14 @@
       </c>
       <c r="K33" s="48"/>
       <c r="L33" s="52"/>
-      <c r="M33" s="156"/>
-      <c r="N33" s="157"/>
-      <c r="O33" s="150"/>
-      <c r="P33" s="151"/>
-      <c r="Q33" s="150">
+      <c r="M33" s="140"/>
+      <c r="N33" s="141"/>
+      <c r="O33" s="138"/>
+      <c r="P33" s="139"/>
+      <c r="Q33" s="138">
         <v>0</v>
       </c>
-      <c r="R33" s="151"/>
+      <c r="R33" s="139"/>
       <c r="S33" s="106"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -2888,14 +2885,14 @@
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
       <c r="L34" s="52"/>
-      <c r="M34" s="152"/>
-      <c r="N34" s="153"/>
-      <c r="O34" s="154"/>
-      <c r="P34" s="155"/>
-      <c r="Q34" s="150">
+      <c r="M34" s="142"/>
+      <c r="N34" s="143"/>
+      <c r="O34" s="144"/>
+      <c r="P34" s="145"/>
+      <c r="Q34" s="138">
         <v>0</v>
       </c>
-      <c r="R34" s="151"/>
+      <c r="R34" s="139"/>
       <c r="S34" s="106"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -2913,14 +2910,14 @@
       <c r="J35" s="48"/>
       <c r="K35" s="48"/>
       <c r="L35" s="48"/>
-      <c r="M35" s="146"/>
-      <c r="N35" s="147"/>
-      <c r="O35" s="148"/>
-      <c r="P35" s="149"/>
-      <c r="Q35" s="150">
+      <c r="M35" s="150"/>
+      <c r="N35" s="151"/>
+      <c r="O35" s="152"/>
+      <c r="P35" s="153"/>
+      <c r="Q35" s="138">
         <v>0</v>
       </c>
-      <c r="R35" s="151"/>
+      <c r="R35" s="139"/>
       <c r="S35" s="106"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -2938,14 +2935,14 @@
       <c r="J36" s="48"/>
       <c r="K36" s="48"/>
       <c r="L36" s="48"/>
-      <c r="M36" s="152"/>
-      <c r="N36" s="153"/>
-      <c r="O36" s="154"/>
-      <c r="P36" s="155"/>
-      <c r="Q36" s="150">
+      <c r="M36" s="142"/>
+      <c r="N36" s="143"/>
+      <c r="O36" s="144"/>
+      <c r="P36" s="145"/>
+      <c r="Q36" s="138">
         <v>0</v>
       </c>
-      <c r="R36" s="151"/>
+      <c r="R36" s="139"/>
       <c r="S36" s="106"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -2963,14 +2960,14 @@
       <c r="J37" s="48"/>
       <c r="K37" s="48"/>
       <c r="L37" s="48"/>
-      <c r="M37" s="146"/>
-      <c r="N37" s="147"/>
-      <c r="O37" s="148"/>
-      <c r="P37" s="149"/>
-      <c r="Q37" s="150">
+      <c r="M37" s="150"/>
+      <c r="N37" s="151"/>
+      <c r="O37" s="152"/>
+      <c r="P37" s="153"/>
+      <c r="Q37" s="138">
         <v>0</v>
       </c>
-      <c r="R37" s="151"/>
+      <c r="R37" s="139"/>
       <c r="S37" s="106"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -2988,14 +2985,14 @@
       <c r="J38" s="48"/>
       <c r="K38" s="48"/>
       <c r="L38" s="48"/>
-      <c r="M38" s="152"/>
-      <c r="N38" s="153"/>
-      <c r="O38" s="154"/>
-      <c r="P38" s="155"/>
-      <c r="Q38" s="150">
+      <c r="M38" s="142"/>
+      <c r="N38" s="143"/>
+      <c r="O38" s="144"/>
+      <c r="P38" s="145"/>
+      <c r="Q38" s="138">
         <v>0</v>
       </c>
-      <c r="R38" s="151"/>
+      <c r="R38" s="139"/>
       <c r="S38" s="106"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -3013,14 +3010,14 @@
       <c r="J39" s="48"/>
       <c r="K39" s="48"/>
       <c r="L39" s="48"/>
-      <c r="M39" s="146"/>
-      <c r="N39" s="147"/>
-      <c r="O39" s="148"/>
-      <c r="P39" s="149"/>
-      <c r="Q39" s="150">
+      <c r="M39" s="150"/>
+      <c r="N39" s="151"/>
+      <c r="O39" s="152"/>
+      <c r="P39" s="153"/>
+      <c r="Q39" s="138">
         <v>0</v>
       </c>
-      <c r="R39" s="151"/>
+      <c r="R39" s="139"/>
       <c r="S39" s="106"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -3038,14 +3035,14 @@
       <c r="J40" s="48"/>
       <c r="K40" s="48"/>
       <c r="L40" s="48"/>
-      <c r="M40" s="146"/>
-      <c r="N40" s="147"/>
-      <c r="O40" s="148"/>
-      <c r="P40" s="149"/>
-      <c r="Q40" s="150">
+      <c r="M40" s="150"/>
+      <c r="N40" s="151"/>
+      <c r="O40" s="152"/>
+      <c r="P40" s="153"/>
+      <c r="Q40" s="138">
         <v>0</v>
       </c>
-      <c r="R40" s="151"/>
+      <c r="R40" s="139"/>
       <c r="S40" s="106"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -3063,14 +3060,14 @@
       <c r="J41" s="57"/>
       <c r="K41" s="57"/>
       <c r="L41" s="58"/>
-      <c r="M41" s="146"/>
-      <c r="N41" s="147"/>
-      <c r="O41" s="148"/>
-      <c r="P41" s="149"/>
-      <c r="Q41" s="150">
+      <c r="M41" s="150"/>
+      <c r="N41" s="151"/>
+      <c r="O41" s="152"/>
+      <c r="P41" s="153"/>
+      <c r="Q41" s="138">
         <v>0</v>
       </c>
-      <c r="R41" s="151"/>
+      <c r="R41" s="139"/>
       <c r="S41" s="106"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -3090,12 +3087,12 @@
       <c r="J42" s="59"/>
       <c r="K42" s="59"/>
       <c r="L42" s="59"/>
-      <c r="M42" s="152"/>
-      <c r="N42" s="153"/>
-      <c r="O42" s="154"/>
-      <c r="P42" s="155"/>
-      <c r="Q42" s="154"/>
-      <c r="R42" s="155"/>
+      <c r="M42" s="142"/>
+      <c r="N42" s="143"/>
+      <c r="O42" s="144"/>
+      <c r="P42" s="145"/>
+      <c r="Q42" s="144"/>
+      <c r="R42" s="145"/>
       <c r="S42" s="106"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -3115,35 +3112,35 @@
       <c r="J43" s="63"/>
       <c r="K43" s="63"/>
       <c r="L43" s="64"/>
-      <c r="M43" s="137" t="s">
+      <c r="M43" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="N43" s="138"/>
-      <c r="O43" s="139" t="s">
-        <v>65</v>
-      </c>
-      <c r="P43" s="140"/>
-      <c r="Q43" s="139" t="s">
-        <v>66</v>
-      </c>
-      <c r="R43" s="140"/>
+      <c r="N43" s="155"/>
+      <c r="O43" s="156">
+        <v>0</v>
+      </c>
+      <c r="P43" s="157"/>
+      <c r="Q43" s="156">
+        <v>0</v>
+      </c>
+      <c r="R43" s="157"/>
       <c r="S43" s="106"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
       <c r="B44" s="47"/>
-      <c r="C44" s="121" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="121"/>
-      <c r="E44" s="121"/>
-      <c r="F44" s="121"/>
-      <c r="G44" s="121"/>
-      <c r="H44" s="121"/>
-      <c r="I44" s="121"/>
-      <c r="J44" s="121"/>
-      <c r="K44" s="121"/>
-      <c r="L44" s="141"/>
+      <c r="C44" s="158" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="158"/>
+      <c r="E44" s="158"/>
+      <c r="F44" s="158"/>
+      <c r="G44" s="158"/>
+      <c r="H44" s="158"/>
+      <c r="I44" s="158"/>
+      <c r="J44" s="158"/>
+      <c r="K44" s="158"/>
+      <c r="L44" s="159"/>
       <c r="M44" s="65"/>
       <c r="N44" s="66"/>
       <c r="O44" s="65"/>
@@ -3155,16 +3152,16 @@
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
       <c r="B45" s="47"/>
-      <c r="C45" s="121"/>
-      <c r="D45" s="121"/>
-      <c r="E45" s="121"/>
-      <c r="F45" s="121"/>
-      <c r="G45" s="121"/>
-      <c r="H45" s="121"/>
-      <c r="I45" s="121"/>
-      <c r="J45" s="121"/>
-      <c r="K45" s="121"/>
-      <c r="L45" s="141"/>
+      <c r="C45" s="158"/>
+      <c r="D45" s="158"/>
+      <c r="E45" s="158"/>
+      <c r="F45" s="158"/>
+      <c r="G45" s="158"/>
+      <c r="H45" s="158"/>
+      <c r="I45" s="158"/>
+      <c r="J45" s="158"/>
+      <c r="K45" s="158"/>
+      <c r="L45" s="159"/>
       <c r="M45" s="35"/>
       <c r="N45" s="36"/>
       <c r="O45" s="35"/>
@@ -3176,16 +3173,16 @@
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
       <c r="B46" s="47"/>
-      <c r="C46" s="121"/>
-      <c r="D46" s="121"/>
-      <c r="E46" s="121"/>
-      <c r="F46" s="121"/>
-      <c r="G46" s="121"/>
-      <c r="H46" s="121"/>
-      <c r="I46" s="121"/>
-      <c r="J46" s="121"/>
-      <c r="K46" s="121"/>
-      <c r="L46" s="141"/>
+      <c r="C46" s="158"/>
+      <c r="D46" s="158"/>
+      <c r="E46" s="158"/>
+      <c r="F46" s="158"/>
+      <c r="G46" s="158"/>
+      <c r="H46" s="158"/>
+      <c r="I46" s="158"/>
+      <c r="J46" s="158"/>
+      <c r="K46" s="158"/>
+      <c r="L46" s="159"/>
       <c r="M46" s="35"/>
       <c r="N46" s="36"/>
       <c r="O46" s="35"/>
@@ -3197,10 +3194,10 @@
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
       <c r="B47" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="22" t="s">
         <v>68</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>69</v>
       </c>
       <c r="D47" s="67"/>
       <c r="E47" s="48"/>
@@ -3211,12 +3208,12 @@
       <c r="J47" s="57"/>
       <c r="K47" s="57"/>
       <c r="L47" s="57"/>
-      <c r="M47" s="142"/>
-      <c r="N47" s="143"/>
-      <c r="O47" s="144"/>
-      <c r="P47" s="145"/>
-      <c r="Q47" s="144"/>
-      <c r="R47" s="145"/>
+      <c r="M47" s="146"/>
+      <c r="N47" s="147"/>
+      <c r="O47" s="148"/>
+      <c r="P47" s="149"/>
+      <c r="Q47" s="148"/>
+      <c r="R47" s="149"/>
       <c r="S47" s="106"/>
     </row>
     <row r="48" spans="1:19" ht="4.3499999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3255,16 +3252,16 @@
       <c r="L49" s="73"/>
       <c r="M49" s="73"/>
       <c r="N49" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="O49" s="110" t="s">
-        <v>65</v>
-      </c>
-      <c r="P49" s="111"/>
-      <c r="Q49" s="110" t="s">
-        <v>66</v>
-      </c>
-      <c r="R49" s="111"/>
+        <v>69</v>
+      </c>
+      <c r="O49" s="162">
+        <v>0</v>
+      </c>
+      <c r="P49" s="163"/>
+      <c r="Q49" s="162">
+        <v>0</v>
+      </c>
+      <c r="R49" s="163"/>
       <c r="S49" s="106"/>
     </row>
     <row r="50" spans="1:19" ht="4.3499999999999996" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -3291,7 +3288,7 @@
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
       <c r="B51" s="81" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C51" s="27"/>
       <c r="D51" s="82"/>
@@ -3299,18 +3296,18 @@
       <c r="F51" s="27"/>
       <c r="G51" s="27"/>
       <c r="H51" s="27"/>
-      <c r="I51" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="J51" s="112"/>
-      <c r="K51" s="112"/>
-      <c r="L51" s="112"/>
-      <c r="M51" s="112"/>
-      <c r="N51" s="112"/>
-      <c r="O51" s="112"/>
-      <c r="P51" s="112"/>
-      <c r="Q51" s="112"/>
-      <c r="R51" s="113"/>
+      <c r="I51" s="164" t="s">
+        <v>71</v>
+      </c>
+      <c r="J51" s="164"/>
+      <c r="K51" s="164"/>
+      <c r="L51" s="164"/>
+      <c r="M51" s="164"/>
+      <c r="N51" s="164"/>
+      <c r="O51" s="164"/>
+      <c r="P51" s="164"/>
+      <c r="Q51" s="164"/>
+      <c r="R51" s="165"/>
       <c r="S51" s="106"/>
     </row>
     <row r="52" spans="1:19" ht="4.3499999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3336,25 +3333,25 @@
     </row>
     <row r="53" spans="1:19" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A53" s="7"/>
-      <c r="B53" s="114" t="s">
-        <v>73</v>
-      </c>
-      <c r="C53" s="115"/>
-      <c r="D53" s="115"/>
-      <c r="E53" s="115"/>
-      <c r="F53" s="115"/>
-      <c r="G53" s="115"/>
-      <c r="H53" s="115"/>
-      <c r="I53" s="115"/>
-      <c r="J53" s="115"/>
-      <c r="K53" s="115"/>
-      <c r="L53" s="115"/>
-      <c r="M53" s="115"/>
-      <c r="N53" s="115"/>
-      <c r="O53" s="115"/>
-      <c r="P53" s="115"/>
-      <c r="Q53" s="115"/>
-      <c r="R53" s="116"/>
+      <c r="B53" s="166" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" s="167"/>
+      <c r="D53" s="167"/>
+      <c r="E53" s="167"/>
+      <c r="F53" s="167"/>
+      <c r="G53" s="167"/>
+      <c r="H53" s="167"/>
+      <c r="I53" s="167"/>
+      <c r="J53" s="167"/>
+      <c r="K53" s="167"/>
+      <c r="L53" s="167"/>
+      <c r="M53" s="167"/>
+      <c r="N53" s="167"/>
+      <c r="O53" s="167"/>
+      <c r="P53" s="167"/>
+      <c r="Q53" s="167"/>
+      <c r="R53" s="168"/>
       <c r="S53" s="105"/>
     </row>
     <row r="54" spans="1:19" ht="4.3499999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3381,7 +3378,7 @@
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="84" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C55" s="85"/>
       <c r="D55" s="85"/>
@@ -3395,12 +3392,12 @@
       <c r="L55" s="85"/>
       <c r="M55" s="85"/>
       <c r="N55" s="85"/>
-      <c r="O55" s="117" t="s">
-        <v>75</v>
-      </c>
-      <c r="P55" s="117"/>
-      <c r="Q55" s="117"/>
-      <c r="R55" s="118"/>
+      <c r="O55" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="P55" s="169"/>
+      <c r="Q55" s="169"/>
+      <c r="R55" s="170"/>
       <c r="S55" s="105"/>
     </row>
     <row r="56" spans="1:19" ht="4.3499999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3427,28 +3424,28 @@
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="87" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C57" s="88"/>
       <c r="D57" s="88"/>
-      <c r="E57" s="119" t="s">
+      <c r="E57" s="171" t="s">
+        <v>76</v>
+      </c>
+      <c r="F57" s="171"/>
+      <c r="G57" s="171"/>
+      <c r="H57" s="171"/>
+      <c r="I57" s="171"/>
+      <c r="J57" s="172"/>
+      <c r="K57" s="176" t="s">
         <v>77</v>
       </c>
-      <c r="F57" s="119"/>
-      <c r="G57" s="119"/>
-      <c r="H57" s="119"/>
-      <c r="I57" s="119"/>
-      <c r="J57" s="120"/>
-      <c r="K57" s="125" t="s">
-        <v>78</v>
-      </c>
-      <c r="L57" s="126"/>
-      <c r="M57" s="126"/>
-      <c r="N57" s="126"/>
-      <c r="O57" s="126"/>
-      <c r="P57" s="126"/>
-      <c r="Q57" s="126"/>
-      <c r="R57" s="127"/>
+      <c r="L57" s="177"/>
+      <c r="M57" s="177"/>
+      <c r="N57" s="177"/>
+      <c r="O57" s="177"/>
+      <c r="P57" s="177"/>
+      <c r="Q57" s="177"/>
+      <c r="R57" s="178"/>
       <c r="S57" s="105"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
@@ -3456,22 +3453,22 @@
       <c r="B58" s="89"/>
       <c r="C58" s="54"/>
       <c r="D58" s="54"/>
-      <c r="E58" s="121"/>
-      <c r="F58" s="121"/>
-      <c r="G58" s="121"/>
-      <c r="H58" s="121"/>
-      <c r="I58" s="121"/>
-      <c r="J58" s="122"/>
-      <c r="K58" s="128" t="s">
-        <v>79</v>
-      </c>
-      <c r="L58" s="129"/>
-      <c r="M58" s="129"/>
-      <c r="N58" s="129"/>
-      <c r="O58" s="129"/>
-      <c r="P58" s="129"/>
-      <c r="Q58" s="129"/>
-      <c r="R58" s="130"/>
+      <c r="E58" s="158"/>
+      <c r="F58" s="158"/>
+      <c r="G58" s="158"/>
+      <c r="H58" s="158"/>
+      <c r="I58" s="158"/>
+      <c r="J58" s="173"/>
+      <c r="K58" s="179" t="s">
+        <v>78</v>
+      </c>
+      <c r="L58" s="180"/>
+      <c r="M58" s="180"/>
+      <c r="N58" s="180"/>
+      <c r="O58" s="180"/>
+      <c r="P58" s="180"/>
+      <c r="Q58" s="180"/>
+      <c r="R58" s="181"/>
       <c r="S58" s="105"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
@@ -3479,22 +3476,22 @@
       <c r="B59" s="89"/>
       <c r="C59" s="54"/>
       <c r="D59" s="54"/>
-      <c r="E59" s="121"/>
-      <c r="F59" s="121"/>
-      <c r="G59" s="121"/>
-      <c r="H59" s="121"/>
-      <c r="I59" s="121"/>
-      <c r="J59" s="122"/>
-      <c r="K59" s="131" t="s">
-        <v>80</v>
-      </c>
-      <c r="L59" s="132"/>
-      <c r="M59" s="132"/>
-      <c r="N59" s="132"/>
-      <c r="O59" s="132"/>
-      <c r="P59" s="132"/>
-      <c r="Q59" s="132"/>
-      <c r="R59" s="133"/>
+      <c r="E59" s="158"/>
+      <c r="F59" s="158"/>
+      <c r="G59" s="158"/>
+      <c r="H59" s="158"/>
+      <c r="I59" s="158"/>
+      <c r="J59" s="173"/>
+      <c r="K59" s="182" t="s">
+        <v>79</v>
+      </c>
+      <c r="L59" s="183"/>
+      <c r="M59" s="183"/>
+      <c r="N59" s="183"/>
+      <c r="O59" s="183"/>
+      <c r="P59" s="183"/>
+      <c r="Q59" s="183"/>
+      <c r="R59" s="184"/>
       <c r="S59" s="105"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
@@ -3502,22 +3499,22 @@
       <c r="B60" s="90"/>
       <c r="C60" s="91"/>
       <c r="D60" s="91"/>
-      <c r="E60" s="123"/>
-      <c r="F60" s="123"/>
-      <c r="G60" s="123"/>
-      <c r="H60" s="123"/>
-      <c r="I60" s="123"/>
-      <c r="J60" s="124"/>
-      <c r="K60" s="134" t="s">
-        <v>81</v>
-      </c>
-      <c r="L60" s="135"/>
-      <c r="M60" s="135"/>
-      <c r="N60" s="135"/>
-      <c r="O60" s="135"/>
-      <c r="P60" s="135"/>
-      <c r="Q60" s="135"/>
-      <c r="R60" s="136"/>
+      <c r="E60" s="174"/>
+      <c r="F60" s="174"/>
+      <c r="G60" s="174"/>
+      <c r="H60" s="174"/>
+      <c r="I60" s="174"/>
+      <c r="J60" s="175"/>
+      <c r="K60" s="185" t="s">
+        <v>80</v>
+      </c>
+      <c r="L60" s="186"/>
+      <c r="M60" s="186"/>
+      <c r="N60" s="186"/>
+      <c r="O60" s="186"/>
+      <c r="P60" s="186"/>
+      <c r="Q60" s="186"/>
+      <c r="R60" s="187"/>
       <c r="S60" s="105"/>
     </row>
     <row r="61" spans="1:19" ht="4.3499999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3575,13 +3572,13 @@
       <c r="J63" s="97"/>
       <c r="K63" s="97"/>
       <c r="L63" s="97"/>
-      <c r="M63" s="108" t="s">
-        <v>80</v>
-      </c>
-      <c r="N63" s="108"/>
-      <c r="O63" s="108"/>
-      <c r="P63" s="108"/>
-      <c r="Q63" s="108"/>
+      <c r="M63" s="160" t="s">
+        <v>79</v>
+      </c>
+      <c r="N63" s="160"/>
+      <c r="O63" s="160"/>
+      <c r="P63" s="160"/>
+      <c r="Q63" s="160"/>
       <c r="R63" s="95"/>
       <c r="S63" s="95"/>
     </row>
@@ -3658,7 +3655,7 @@
       <c r="E67" s="95"/>
       <c r="F67" s="95"/>
       <c r="G67" s="102" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H67" s="95"/>
       <c r="I67" s="95"/>
@@ -3686,11 +3683,11 @@
       <c r="J68" s="95"/>
       <c r="K68" s="95"/>
       <c r="L68" s="95"/>
-      <c r="M68" s="109" t="s">
+      <c r="M68" s="161" t="s">
         <v>65</v>
       </c>
-      <c r="N68" s="109"/>
-      <c r="O68" s="109"/>
+      <c r="N68" s="161"/>
+      <c r="O68" s="161"/>
       <c r="P68" s="103"/>
       <c r="Q68" s="103"/>
       <c r="R68" s="95"/>
@@ -3698,84 +3695,6 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="B21:L22"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P22"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="B4:P4"/>
-    <mergeCell ref="D6:L6"/>
-    <mergeCell ref="D8:R8"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="O39:P39"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="C44:L46"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="O47:P47"/>
-    <mergeCell ref="Q47:R47"/>
     <mergeCell ref="M63:Q63"/>
     <mergeCell ref="M68:O68"/>
     <mergeCell ref="O49:P49"/>
@@ -3788,6 +3707,84 @@
     <mergeCell ref="K58:R58"/>
     <mergeCell ref="K59:R59"/>
     <mergeCell ref="K60:R60"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="C44:L46"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:P4"/>
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="D8:R8"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B21:L22"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P22"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="Q22:R22"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>